<commit_message>
Initial commit 5-6-2022 Office framework
</commit_message>
<xml_diff>
--- a/test_data/Credentials.xlsx
+++ b/test_data/Credentials.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MANSI\eclipse-workspace\FrameworkDemo\test_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F083370B-ED4C-4CF8-964E-2258F336217A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SignUp" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,18 +19,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>qbankadmin</t>
-  </si>
-  <si>
-    <t>pass123</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>jerry1yopmail.com</t>
+  </si>
+  <si>
+    <t>InvalidEmail</t>
+  </si>
+  <si>
+    <t>ValidEmail</t>
+  </si>
+  <si>
+    <t>ExistEmail</t>
+  </si>
+  <si>
+    <t>derbi@yopmail.com</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Company name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm password</t>
+  </si>
+  <si>
+    <t>jerry</t>
+  </si>
+  <si>
+    <t>Graphic designing</t>
+  </si>
+  <si>
+    <t>jerry2@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -129,7 +153,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -164,7 +188,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -341,31 +365,74 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>11111111</v>
+      </c>
+      <c r="G2">
+        <v>11111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Verify the build is trigger or not
</commit_message>
<xml_diff>
--- a/test_data/Credentials.xlsx
+++ b/test_data/Credentials.xlsx
@@ -54,7 +54,7 @@
     <t>Graphic designing</t>
   </si>
   <si>
-    <t>jerry2@yopmail.com</t>
+    <t>jerry3@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -365,7 +365,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -376,7 +376,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated code Date 6 and 6PM
</commit_message>
<xml_diff>
--- a/test_data/Credentials.xlsx
+++ b/test_data/Credentials.xlsx
@@ -54,17 +54,25 @@
     <t>Graphic designing</t>
   </si>
   <si>
-    <t>jerry3@yopmail.com</t>
+    <t>jerry4@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,14 +95,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -365,7 +376,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -376,7 +387,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +430,7 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
@@ -436,7 +447,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit with configured 7-5-2022
</commit_message>
<xml_diff>
--- a/test_data/Credentials.xlsx
+++ b/test_data/Credentials.xlsx
@@ -54,7 +54,7 @@
     <t>Graphic designing</t>
   </si>
   <si>
-    <t>jerry5@yopmail.com</t>
+    <t>jerry6@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -365,7 +365,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -376,7 +376,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Commit with latest configuration 7-5-2022
</commit_message>
<xml_diff>
--- a/test_data/Credentials.xlsx
+++ b/test_data/Credentials.xlsx
@@ -54,7 +54,7 @@
     <t>Graphic designing</t>
   </si>
   <si>
-    <t>jerry7@yopmail.com</t>
+    <t>davidkamroo@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -365,7 +365,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -376,7 +376,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Verified the sign up test cases which I created before. (29-05-2022)
</commit_message>
<xml_diff>
--- a/test_data/Credentials.xlsx
+++ b/test_data/Credentials.xlsx
@@ -54,7 +54,7 @@
     <t>Graphic designing</t>
   </si>
   <si>
-    <t>davidkamroo@yopmail.com</t>
+    <t>davidkamroo1@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -365,7 +365,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -376,7 +376,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D14" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>